<commit_message>
fix FY input range
</commit_message>
<xml_diff>
--- a/FCF_Analysis_Temp1.xlsx
+++ b/FCF_Analysis_Temp1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AsusWebStorage\ran@benhur.co\MySyncFolder\RaniStuff\IBI\Stock Analysis\Financials\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AsusWebStorage\ran@benhur.co\MySyncFolder\python\investingAnalysis\financial_to_exel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B540E88C-C02D-44EF-B8C7-8D946AF9EBDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50CF032B-85B3-44E4-ACAC-C39092318950}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -109,7 +109,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="73">
   <si>
     <t>date of Analysis</t>
   </si>
@@ -120,9 +120,6 @@
     <t>Period End Date</t>
   </si>
   <si>
-    <t>2024-09-30</t>
-  </si>
-  <si>
     <t>Income Statement</t>
   </si>
   <si>
@@ -172,33 +169,6 @@
   </si>
   <si>
     <t>Cash from Financing</t>
-  </si>
-  <si>
-    <t>2015-12-31</t>
-  </si>
-  <si>
-    <t>2016-12-31</t>
-  </si>
-  <si>
-    <t>2017-12-31</t>
-  </si>
-  <si>
-    <t>2018-12-31</t>
-  </si>
-  <si>
-    <t>2019-12-31</t>
-  </si>
-  <si>
-    <t>2020-12-31</t>
-  </si>
-  <si>
-    <t>2021-12-31</t>
-  </si>
-  <si>
-    <t>2022-12-31</t>
-  </si>
-  <si>
-    <t>2023-12-31</t>
   </si>
   <si>
     <t>Chart Title</t>
@@ -1136,31 +1106,31 @@
     <xf numFmtId="166" fontId="0" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1294,42 +1264,43 @@
             </c:spPr>
           </c:marker>
           <c:xVal>
-            <c:strRef>
+            <c:numRef>
               <c:f>'FCF DATA'!$B$3:$B$12</c:f>
-              <c:strCache>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>2015-12-31</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2016-12-31</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2017-12-31</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2018-12-31</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2019-12-31</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2020-12-31</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2021-12-31</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2022-12-31</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2023-12-31</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2024-09-30</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
@@ -1416,42 +1387,43 @@
             </c:spPr>
           </c:marker>
           <c:xVal>
-            <c:strRef>
+            <c:numRef>
               <c:f>'FCF DATA'!$B$18:$B$27</c:f>
-              <c:strCache>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>2015-12-31</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2016-12-31</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2017-12-31</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2018-12-31</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2019-12-31</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2020-12-31</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2021-12-31</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2022-12-31</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2023-12-31</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2024-09-30</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
@@ -1538,42 +1510,43 @@
             </c:spPr>
           </c:marker>
           <c:xVal>
-            <c:strRef>
+            <c:numRef>
               <c:f>'FCF DATA'!$B$35:$B$44</c:f>
-              <c:strCache>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>2015-12-31</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2016-12-31</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2017-12-31</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2018-12-31</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2019-12-31</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2020-12-31</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2021-12-31</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2022-12-31</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2023-12-31</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2024-09-30</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
@@ -1660,42 +1633,43 @@
             </c:spPr>
           </c:marker>
           <c:xVal>
-            <c:strRef>
+            <c:numRef>
               <c:f>'FCF DATA'!$B$50:$B$59</c:f>
-              <c:strCache>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>2015-12-31</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2016-12-31</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2017-12-31</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2018-12-31</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2019-12-31</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2020-12-31</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2021-12-31</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2022-12-31</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2023-12-31</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2024-09-30</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
@@ -2019,39 +1993,40 @@
             </c:spPr>
           </c:marker>
           <c:xVal>
-            <c:strRef>
+            <c:numRef>
               <c:f>'FCF DATA'!$B$64:$B$72</c:f>
-              <c:strCache>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>2015-12-31</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2016-12-31</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2017-12-31</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2018-12-31</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2019-12-31</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2020-12-31</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2021-12-31</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2022-12-31</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2023-12-31</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
@@ -2135,39 +2110,40 @@
             </c:spPr>
           </c:marker>
           <c:xVal>
-            <c:strRef>
+            <c:numRef>
               <c:f>'FCF DATA'!$B$64:$B$72</c:f>
-              <c:strCache>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>2015-12-31</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2016-12-31</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2017-12-31</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2018-12-31</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2019-12-31</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2020-12-31</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2021-12-31</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2022-12-31</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2023-12-31</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
@@ -2251,39 +2227,40 @@
             </c:spPr>
           </c:marker>
           <c:xVal>
-            <c:strRef>
+            <c:numRef>
               <c:f>'FCF DATA'!$B$64:$B$72</c:f>
-              <c:strCache>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>2015-12-31</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2016-12-31</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2017-12-31</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2018-12-31</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2019-12-31</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2020-12-31</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2021-12-31</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2022-12-31</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2023-12-31</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
@@ -2367,39 +2344,40 @@
             </c:spPr>
           </c:marker>
           <c:xVal>
-            <c:strRef>
+            <c:numRef>
               <c:f>'FCF DATA'!$B$64:$B$72</c:f>
-              <c:strCache>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>2015-12-31</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2016-12-31</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2017-12-31</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2018-12-31</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2019-12-31</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2020-12-31</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2021-12-31</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2022-12-31</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2023-12-31</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
@@ -2637,7 +2615,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="113" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="118" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -2648,7 +2626,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="112" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="118" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -2659,7 +2637,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9297412" cy="6043739"/>
+    <xdr:ext cx="9298983" cy="6045953"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -2692,7 +2670,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9295379" cy="6046674"/>
+    <xdr:ext cx="9298983" cy="6045953"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -3109,7 +3087,7 @@
   <dimension ref="A1:O23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3151,22 +3129,22 @@
     <row r="4" spans="1:15" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="1:15" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="73" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C5" s="74"/>
       <c r="D5" s="74"/>
       <c r="E5" s="74"/>
       <c r="F5" s="75"/>
       <c r="G5" s="73" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H5" s="75"/>
       <c r="I5" s="73" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J5" s="75"/>
       <c r="K5" s="73" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="L5" s="74"/>
       <c r="M5" s="74"/>
@@ -3178,52 +3156,50 @@
         <v>2</v>
       </c>
       <c r="B6" s="87" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="88" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="88" t="s">
+      <c r="D6" s="88" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="88" t="s">
+      <c r="E6" s="89" t="s">
         <v>9</v>
       </c>
-      <c r="E6" s="89" t="s">
+      <c r="F6" s="90" t="s">
         <v>10</v>
       </c>
-      <c r="F6" s="90" t="s">
+      <c r="G6" s="91" t="s">
         <v>11</v>
       </c>
-      <c r="G6" s="91" t="s">
+      <c r="H6" s="89" t="s">
         <v>12</v>
       </c>
-      <c r="H6" s="89" t="s">
+      <c r="I6" s="87" t="s">
         <v>13</v>
       </c>
-      <c r="I6" s="87" t="s">
+      <c r="J6" s="93" t="s">
         <v>14</v>
       </c>
-      <c r="J6" s="93" t="s">
+      <c r="K6" s="88" t="s">
         <v>15</v>
       </c>
-      <c r="K6" s="88" t="s">
+      <c r="L6" s="88" t="s">
         <v>16</v>
       </c>
-      <c r="L6" s="88" t="s">
+      <c r="M6" s="89" t="s">
         <v>17</v>
       </c>
-      <c r="M6" s="89" t="s">
+      <c r="N6" s="89" t="s">
         <v>18</v>
       </c>
-      <c r="N6" s="89" t="s">
+      <c r="O6" s="92" t="s">
         <v>19</v>
       </c>
-      <c r="O6" s="92" t="s">
-        <v>20</v>
-      </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A7" s="103" t="s">
-        <v>21</v>
-      </c>
+      <c r="A7" s="103"/>
       <c r="B7" s="76"/>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
@@ -3240,9 +3216,7 @@
       <c r="O7" s="83"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A8" s="103" t="s">
-        <v>22</v>
-      </c>
+      <c r="A8" s="103"/>
       <c r="B8" s="76"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
@@ -3265,9 +3239,7 @@
       <c r="O8" s="83"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A9" s="103" t="s">
-        <v>23</v>
-      </c>
+      <c r="A9" s="103"/>
       <c r="B9" s="76"/>
       <c r="C9" s="95"/>
       <c r="D9" s="2"/>
@@ -3290,9 +3262,7 @@
       <c r="O9" s="83"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A10" s="103" t="s">
-        <v>24</v>
-      </c>
+      <c r="A10" s="103"/>
       <c r="B10" s="76"/>
       <c r="C10" s="95"/>
       <c r="D10" s="2"/>
@@ -3315,9 +3285,7 @@
       <c r="O10" s="83"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A11" s="103" t="s">
-        <v>25</v>
-      </c>
+      <c r="A11" s="103"/>
       <c r="B11" s="76"/>
       <c r="C11" s="95"/>
       <c r="D11" s="2"/>
@@ -3340,9 +3308,7 @@
       <c r="O11" s="83"/>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A12" s="103" t="s">
-        <v>26</v>
-      </c>
+      <c r="A12" s="103"/>
       <c r="B12" s="76"/>
       <c r="C12" s="95"/>
       <c r="D12" s="2"/>
@@ -3365,9 +3331,7 @@
       <c r="O12" s="83"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A13" s="103" t="s">
-        <v>27</v>
-      </c>
+      <c r="A13" s="103"/>
       <c r="B13" s="76"/>
       <c r="C13" s="95"/>
       <c r="D13" s="2"/>
@@ -3390,9 +3354,7 @@
       <c r="O13" s="83"/>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A14" s="103" t="s">
-        <v>28</v>
-      </c>
+      <c r="A14" s="103"/>
       <c r="B14" s="76"/>
       <c r="C14" s="95"/>
       <c r="D14" s="2"/>
@@ -3415,9 +3377,7 @@
       <c r="O14" s="83"/>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A15" s="103" t="s">
-        <v>29</v>
-      </c>
+      <c r="A15" s="103"/>
       <c r="B15" s="76"/>
       <c r="C15" s="95"/>
       <c r="D15" s="2"/>
@@ -3440,9 +3400,7 @@
       <c r="O15" s="83"/>
     </row>
     <row r="16" spans="1:15" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="104" t="s">
-        <v>3</v>
-      </c>
+      <c r="A16" s="104"/>
       <c r="B16" s="79"/>
       <c r="C16" s="96"/>
       <c r="D16" s="96"/>
@@ -3466,12 +3424,12 @@
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.25">
@@ -3535,14 +3493,14 @@
         <f>'FCF DATA'!G49</f>
         <v>Growth</v>
       </c>
-      <c r="F3" s="108" t="s">
-        <v>32</v>
-      </c>
-      <c r="G3" s="109"/>
-      <c r="I3" s="114" t="s">
-        <v>33</v>
-      </c>
-      <c r="J3" s="109"/>
+      <c r="F3" s="110" t="s">
+        <v>22</v>
+      </c>
+      <c r="G3" s="111"/>
+      <c r="I3" s="117" t="s">
+        <v>23</v>
+      </c>
+      <c r="J3" s="111"/>
     </row>
     <row r="4" spans="2:14" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C4" s="8" t="str">
@@ -3554,7 +3512,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="F4" s="10" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="G4" s="100">
         <v>0.12</v>
@@ -3575,7 +3533,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="F5" s="11" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="G5" s="101">
         <v>0.1</v>
@@ -3602,19 +3560,19 @@
         <f>'FCF DATA'!G54</f>
         <v>Min CF + 10%</v>
       </c>
-      <c r="F8" s="108" t="s">
-        <v>36</v>
-      </c>
-      <c r="G8" s="109"/>
-      <c r="I8" s="117" t="s">
-        <v>37</v>
-      </c>
-      <c r="J8" s="109"/>
+      <c r="F8" s="110" t="s">
+        <v>26</v>
+      </c>
+      <c r="G8" s="111"/>
+      <c r="I8" s="112" t="s">
+        <v>27</v>
+      </c>
+      <c r="J8" s="111"/>
     </row>
     <row r="9" spans="2:14" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C9" s="32" t="str">
+      <c r="C9" s="32">
         <f>'FCF DATA'!F55</f>
-        <v>2024-09-30</v>
+        <v>0</v>
       </c>
       <c r="D9" s="33" t="e">
         <f>'FCF DATA'!G55</f>
@@ -3632,7 +3590,7 @@
     <row r="10" spans="2:14" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="11" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B11" s="13" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="C11" s="23">
         <v>0</v>
@@ -3667,63 +3625,63 @@
       <c r="M11" s="14">
         <v>10</v>
       </c>
-      <c r="N11" s="106" t="s">
-        <v>39</v>
+      <c r="N11" s="113" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="12" spans="2:14" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="C12" s="25" t="str">
+        <v>30</v>
+      </c>
+      <c r="C12" s="25">
         <f>C9</f>
-        <v>2024-09-30</v>
+        <v>0</v>
       </c>
       <c r="D12" s="26">
         <f t="shared" ref="D12:M12" si="0">C12+1</f>
-        <v>45566</v>
+        <v>1</v>
       </c>
       <c r="E12" s="26">
         <f t="shared" si="0"/>
-        <v>45567</v>
+        <v>2</v>
       </c>
       <c r="F12" s="26">
         <f t="shared" si="0"/>
-        <v>45568</v>
+        <v>3</v>
       </c>
       <c r="G12" s="26">
         <f t="shared" si="0"/>
-        <v>45569</v>
+        <v>4</v>
       </c>
       <c r="H12" s="26">
         <f t="shared" si="0"/>
-        <v>45570</v>
+        <v>5</v>
       </c>
       <c r="I12" s="26">
         <f t="shared" si="0"/>
-        <v>45571</v>
+        <v>6</v>
       </c>
       <c r="J12" s="26">
         <f t="shared" si="0"/>
-        <v>45572</v>
+        <v>7</v>
       </c>
       <c r="K12" s="26">
         <f t="shared" si="0"/>
-        <v>45573</v>
+        <v>8</v>
       </c>
       <c r="L12" s="26">
         <f t="shared" si="0"/>
-        <v>45574</v>
+        <v>9</v>
       </c>
       <c r="M12" s="22">
         <f t="shared" si="0"/>
-        <v>45575</v>
-      </c>
-      <c r="N12" s="107"/>
+        <v>10</v>
+      </c>
+      <c r="N12" s="114"/>
     </row>
     <row r="13" spans="2:14" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B13" s="13" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="C13" s="40" t="e">
         <f>D9</f>
@@ -3775,10 +3733,10 @@
       </c>
     </row>
     <row r="14" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B14" s="112" t="s">
-        <v>42</v>
-      </c>
-      <c r="C14" s="113"/>
+      <c r="B14" s="108" t="s">
+        <v>32</v>
+      </c>
+      <c r="C14" s="109"/>
       <c r="D14" s="16">
         <f>$G$4</f>
         <v>0.12</v>
@@ -3822,10 +3780,10 @@
       <c r="N14" s="12"/>
     </row>
     <row r="15" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B15" s="112" t="s">
-        <v>43</v>
-      </c>
-      <c r="C15" s="113"/>
+      <c r="B15" s="108" t="s">
+        <v>33</v>
+      </c>
+      <c r="C15" s="109"/>
       <c r="D15" s="17">
         <f t="shared" ref="D15:M15" si="2">(1+$G$9)^D11</f>
         <v>1.1000000000000001</v>
@@ -3869,10 +3827,10 @@
       <c r="N15" s="12"/>
     </row>
     <row r="16" spans="2:14" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="110" t="s">
-        <v>44</v>
-      </c>
-      <c r="C16" s="111"/>
+      <c r="B16" s="115" t="s">
+        <v>34</v>
+      </c>
+      <c r="C16" s="116"/>
       <c r="D16" s="20" t="e">
         <f t="shared" ref="D16:M16" si="3">D13/D15</f>
         <v>#DIV/0!</v>
@@ -3938,15 +3896,15 @@
       <c r="D18" s="38"/>
     </row>
     <row r="19" spans="2:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C19" s="115" t="e" vm="4">
+      <c r="C19" s="106" t="e" vm="4">
         <f t="array" ref="C19">_FV('Data Entry'!C2,"Official name",TRUE)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="D19" s="116"/>
+      <c r="D19" s="107"/>
     </row>
     <row r="20" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C20" s="27" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="D20" s="51" t="e" vm="5">
         <f t="array" ref="D20">_FV('Data Entry'!C2,"Price")</f>
@@ -3955,7 +3913,7 @@
     </row>
     <row r="21" spans="2:14" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C21" s="9" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="D21" s="28" t="e" vm="6">
         <f t="array" ref="D21">_FV('Data Entry'!C2,"Shares outstanding",TRUE)</f>
@@ -3965,7 +3923,7 @@
     <row r="22" spans="2:14" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="23" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C23" s="29" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="D23" s="30" t="e">
         <f>SUM(D16:M16)+N13</f>
@@ -3974,7 +3932,7 @@
     </row>
     <row r="24" spans="2:14" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C24" s="31" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="D24" s="52" t="e">
         <f>D23/D21*1000000</f>
@@ -3983,7 +3941,7 @@
     </row>
     <row r="26" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C26" s="72" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="D26" s="71" t="e">
         <f>(D24-D20)/D20</f>
@@ -3992,15 +3950,15 @@
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="I3:J3"/>
     <mergeCell ref="C19:D19"/>
     <mergeCell ref="B14:C14"/>
     <mergeCell ref="F8:G8"/>
     <mergeCell ref="I8:J8"/>
     <mergeCell ref="N11:N12"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="I3:J3"/>
   </mergeCells>
   <conditionalFormatting sqref="D26">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="lessThan">
@@ -4018,8 +3976,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:O72"/>
   <sheetViews>
-    <sheetView topLeftCell="A44" workbookViewId="0">
-      <selection activeCell="G53" sqref="G53"/>
+    <sheetView topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="G52" sqref="G52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4040,34 +3998,34 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C1" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="B2" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="C2" s="45" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="D2" s="49" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="E2" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <f>YEAR(B3)</f>
-        <v>2015</v>
-      </c>
-      <c r="B3" t="str">
+        <v>1900</v>
+      </c>
+      <c r="B3">
         <f t="array" ref="B3:B12">'Data Entry'!A7:A16</f>
-        <v>2015-12-31</v>
+        <v>0</v>
       </c>
       <c r="C3" s="68">
         <f t="array" ref="C3:C12">'Data Entry'!M7:M16</f>
@@ -4085,10 +4043,10 @@
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <f t="shared" ref="A4:A12" si="1">YEAR(B4)</f>
-        <v>2016</v>
-      </c>
-      <c r="B4" t="str">
-        <v>2016-12-31</v>
+        <v>1900</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
       </c>
       <c r="C4" s="68">
         <v>0</v>
@@ -4104,10 +4062,10 @@
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <f t="shared" si="1"/>
-        <v>2017</v>
-      </c>
-      <c r="B5" t="str">
-        <v>2017-12-31</v>
+        <v>1900</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
       </c>
       <c r="C5" s="68">
         <v>0</v>
@@ -4123,10 +4081,10 @@
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <f t="shared" si="1"/>
-        <v>2018</v>
-      </c>
-      <c r="B6" t="str">
-        <v>2018-12-31</v>
+        <v>1900</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
       </c>
       <c r="C6" s="68">
         <v>0</v>
@@ -4142,10 +4100,10 @@
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
         <f t="shared" si="1"/>
-        <v>2019</v>
-      </c>
-      <c r="B7" t="str">
-        <v>2019-12-31</v>
+        <v>1900</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
       </c>
       <c r="C7" s="68">
         <v>0</v>
@@ -4161,10 +4119,10 @@
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
         <f t="shared" si="1"/>
-        <v>2020</v>
-      </c>
-      <c r="B8" t="str">
-        <v>2020-12-31</v>
+        <v>1900</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
       </c>
       <c r="C8" s="68">
         <v>0</v>
@@ -4180,10 +4138,10 @@
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
         <f t="shared" si="1"/>
-        <v>2021</v>
-      </c>
-      <c r="B9" t="str">
-        <v>2021-12-31</v>
+        <v>1900</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
       </c>
       <c r="C9" s="68">
         <v>0</v>
@@ -4199,10 +4157,10 @@
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
         <f t="shared" si="1"/>
-        <v>2022</v>
-      </c>
-      <c r="B10" t="str">
-        <v>2022-12-31</v>
+        <v>1900</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
       </c>
       <c r="C10" s="68">
         <v>0</v>
@@ -4218,10 +4176,10 @@
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
         <f t="shared" si="1"/>
-        <v>2023</v>
-      </c>
-      <c r="B11" t="str">
-        <v>2023-12-31</v>
+        <v>1900</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
       </c>
       <c r="C11" s="68">
         <v>0</v>
@@ -4237,10 +4195,10 @@
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12">
         <f t="shared" si="1"/>
-        <v>2024</v>
-      </c>
-      <c r="B12" t="str">
-        <v>2024-09-30</v>
+        <v>1900</v>
+      </c>
+      <c r="B12">
+        <v>0</v>
       </c>
       <c r="C12" s="68">
         <v>0</v>
@@ -4255,51 +4213,51 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="C14" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="D14" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C16" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="B17" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="C17" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D17" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="E17" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="F17" s="45" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="G17" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18">
         <f>YEAR(B18)</f>
-        <v>2015</v>
-      </c>
-      <c r="B18" t="str">
+        <v>1900</v>
+      </c>
+      <c r="B18">
         <f t="shared" ref="B18:B27" si="2">B3</f>
-        <v>2015-12-31</v>
+        <v>0</v>
       </c>
       <c r="C18" s="2">
         <f t="array" ref="C18:C27">'Data Entry'!F7:F16</f>
@@ -4325,11 +4283,11 @@
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19">
         <f t="shared" ref="A19:A27" si="4">YEAR(B19)</f>
-        <v>2016</v>
-      </c>
-      <c r="B19" t="str">
+        <v>1900</v>
+      </c>
+      <c r="B19">
         <f t="shared" si="2"/>
-        <v>2016-12-31</v>
+        <v>0</v>
       </c>
       <c r="C19" s="2">
         <v>0</v>
@@ -4352,11 +4310,11 @@
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20">
         <f t="shared" si="4"/>
-        <v>2017</v>
-      </c>
-      <c r="B20" t="str">
+        <v>1900</v>
+      </c>
+      <c r="B20">
         <f t="shared" si="2"/>
-        <v>2017-12-31</v>
+        <v>0</v>
       </c>
       <c r="C20" s="2">
         <v>0</v>
@@ -4379,11 +4337,11 @@
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21">
         <f t="shared" si="4"/>
-        <v>2018</v>
-      </c>
-      <c r="B21" t="str">
+        <v>1900</v>
+      </c>
+      <c r="B21">
         <f t="shared" si="2"/>
-        <v>2018-12-31</v>
+        <v>0</v>
       </c>
       <c r="C21" s="2">
         <v>0</v>
@@ -4406,11 +4364,11 @@
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22">
         <f t="shared" si="4"/>
-        <v>2019</v>
-      </c>
-      <c r="B22" t="str">
+        <v>1900</v>
+      </c>
+      <c r="B22">
         <f t="shared" si="2"/>
-        <v>2019-12-31</v>
+        <v>0</v>
       </c>
       <c r="C22" s="2">
         <v>0</v>
@@ -4433,11 +4391,11 @@
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23">
         <f t="shared" si="4"/>
-        <v>2020</v>
-      </c>
-      <c r="B23" t="str">
+        <v>1900</v>
+      </c>
+      <c r="B23">
         <f t="shared" si="2"/>
-        <v>2020-12-31</v>
+        <v>0</v>
       </c>
       <c r="C23" s="2">
         <v>0</v>
@@ -4460,11 +4418,11 @@
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24">
         <f t="shared" si="4"/>
-        <v>2021</v>
-      </c>
-      <c r="B24" t="str">
+        <v>1900</v>
+      </c>
+      <c r="B24">
         <f t="shared" si="2"/>
-        <v>2021-12-31</v>
+        <v>0</v>
       </c>
       <c r="C24" s="2">
         <v>0</v>
@@ -4487,11 +4445,11 @@
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25">
         <f t="shared" si="4"/>
-        <v>2022</v>
-      </c>
-      <c r="B25" t="str">
+        <v>1900</v>
+      </c>
+      <c r="B25">
         <f t="shared" si="2"/>
-        <v>2022-12-31</v>
+        <v>0</v>
       </c>
       <c r="C25" s="2">
         <v>0</v>
@@ -4514,11 +4472,11 @@
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26">
         <f t="shared" si="4"/>
-        <v>2023</v>
-      </c>
-      <c r="B26" t="str">
+        <v>1900</v>
+      </c>
+      <c r="B26">
         <f t="shared" si="2"/>
-        <v>2023-12-31</v>
+        <v>0</v>
       </c>
       <c r="C26" s="2">
         <v>0</v>
@@ -4541,11 +4499,11 @@
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27">
         <f t="shared" si="4"/>
-        <v>2024</v>
-      </c>
-      <c r="B27" t="str">
+        <v>1900</v>
+      </c>
+      <c r="B27">
         <f t="shared" si="2"/>
-        <v>2024-09-30</v>
+        <v>0</v>
       </c>
       <c r="C27" s="2">
         <v>0</v>
@@ -4570,82 +4528,82 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="C29" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="D29" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="E29" s="2"/>
       <c r="F29" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E30" s="4" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C32" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.25">
       <c r="N33" s="47" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="O33" s="47"/>
     </row>
     <row r="34" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="B34" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="C34" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="D34" s="48" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="E34" s="46" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="F34" s="49" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="G34" s="45" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="H34" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="J34" s="48" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="K34" s="48" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="L34" s="48"/>
       <c r="N34" s="45" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="O34" s="45" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A35">
         <f>YEAR(B35)</f>
-        <v>2015</v>
-      </c>
-      <c r="B35" t="str">
+        <v>1900</v>
+      </c>
+      <c r="B35">
         <f t="shared" ref="B35:B44" si="5">B3</f>
-        <v>2015-12-31</v>
+        <v>0</v>
       </c>
       <c r="C35" s="68">
         <f t="array" ref="C35:C44">'Data Entry'!E7:E16</f>
@@ -4689,11 +4647,11 @@
     <row r="36" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A36">
         <f t="shared" ref="A36:A44" si="10">YEAR(B36)</f>
-        <v>2016</v>
-      </c>
-      <c r="B36" t="str">
+        <v>1900</v>
+      </c>
+      <c r="B36">
         <f t="shared" si="5"/>
-        <v>2016-12-31</v>
+        <v>0</v>
       </c>
       <c r="C36" s="68">
         <v>0</v>
@@ -4733,11 +4691,11 @@
     <row r="37" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A37">
         <f t="shared" si="10"/>
-        <v>2017</v>
-      </c>
-      <c r="B37" t="str">
+        <v>1900</v>
+      </c>
+      <c r="B37">
         <f t="shared" si="5"/>
-        <v>2017-12-31</v>
+        <v>0</v>
       </c>
       <c r="C37" s="68">
         <v>0</v>
@@ -4777,11 +4735,11 @@
     <row r="38" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A38">
         <f t="shared" si="10"/>
-        <v>2018</v>
-      </c>
-      <c r="B38" t="str">
+        <v>1900</v>
+      </c>
+      <c r="B38">
         <f t="shared" si="5"/>
-        <v>2018-12-31</v>
+        <v>0</v>
       </c>
       <c r="C38" s="68">
         <v>0</v>
@@ -4821,11 +4779,11 @@
     <row r="39" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A39">
         <f t="shared" si="10"/>
-        <v>2019</v>
-      </c>
-      <c r="B39" t="str">
+        <v>1900</v>
+      </c>
+      <c r="B39">
         <f t="shared" si="5"/>
-        <v>2019-12-31</v>
+        <v>0</v>
       </c>
       <c r="C39" s="68">
         <v>0</v>
@@ -4865,11 +4823,11 @@
     <row r="40" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A40">
         <f t="shared" si="10"/>
-        <v>2020</v>
-      </c>
-      <c r="B40" t="str">
+        <v>1900</v>
+      </c>
+      <c r="B40">
         <f t="shared" si="5"/>
-        <v>2020-12-31</v>
+        <v>0</v>
       </c>
       <c r="C40" s="68">
         <v>0</v>
@@ -4909,11 +4867,11 @@
     <row r="41" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A41">
         <f t="shared" si="10"/>
-        <v>2021</v>
-      </c>
-      <c r="B41" t="str">
+        <v>1900</v>
+      </c>
+      <c r="B41">
         <f t="shared" si="5"/>
-        <v>2021-12-31</v>
+        <v>0</v>
       </c>
       <c r="C41" s="68">
         <v>0</v>
@@ -4953,11 +4911,11 @@
     <row r="42" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A42">
         <f t="shared" si="10"/>
-        <v>2022</v>
-      </c>
-      <c r="B42" t="str">
+        <v>1900</v>
+      </c>
+      <c r="B42">
         <f t="shared" si="5"/>
-        <v>2022-12-31</v>
+        <v>0</v>
       </c>
       <c r="C42" s="68">
         <v>0</v>
@@ -4997,11 +4955,11 @@
     <row r="43" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A43">
         <f t="shared" si="10"/>
-        <v>2023</v>
-      </c>
-      <c r="B43" t="str">
+        <v>1900</v>
+      </c>
+      <c r="B43">
         <f t="shared" si="5"/>
-        <v>2023-12-31</v>
+        <v>0</v>
       </c>
       <c r="C43" s="68">
         <v>0</v>
@@ -5041,11 +4999,11 @@
     <row r="44" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A44">
         <f t="shared" si="10"/>
-        <v>2024</v>
-      </c>
-      <c r="B44" t="str">
+        <v>1900</v>
+      </c>
+      <c r="B44">
         <f t="shared" si="5"/>
-        <v>2024-09-30</v>
+        <v>0</v>
       </c>
       <c r="C44" s="68">
         <v>0</v>
@@ -5084,64 +5042,64 @@
     </row>
     <row r="46" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="C46" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="F46" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="G46" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="J46" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="K46" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="N46" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="O46" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
     </row>
     <row r="47" spans="1:15" x14ac:dyDescent="0.25">
       <c r="G47" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="B49" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="C49" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="G49" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50">
         <f>YEAR(B50)</f>
-        <v>2015</v>
-      </c>
-      <c r="B50" t="str">
+        <v>1900</v>
+      </c>
+      <c r="B50">
         <f t="shared" ref="B50:B59" si="11">B3</f>
-        <v>2015-12-31</v>
+        <v>0</v>
       </c>
       <c r="C50" s="3" t="e">
         <f t="shared" ref="C50:C59" si="12">(E3+G18+H35)/3</f>
         <v>#DIV/0!</v>
       </c>
       <c r="F50" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="G50" s="5" t="e">
         <f>SLOPE(C56:C59,A56:A59)/C56/3</f>
@@ -5151,18 +5109,18 @@
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51">
         <f t="shared" ref="A51:A59" si="13">YEAR(B51)</f>
-        <v>2016</v>
-      </c>
-      <c r="B51" t="str">
+        <v>1900</v>
+      </c>
+      <c r="B51">
         <f t="shared" si="11"/>
-        <v>2016-12-31</v>
+        <v>0</v>
       </c>
       <c r="C51" s="3" t="e">
         <f t="shared" si="12"/>
         <v>#DIV/0!</v>
       </c>
       <c r="F51" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="G51" s="5" t="e">
         <f>SLOPE(C54:C59,A54:A59)/C54/5</f>
@@ -5172,18 +5130,18 @@
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52">
         <f t="shared" si="13"/>
-        <v>2017</v>
-      </c>
-      <c r="B52" t="str">
+        <v>1900</v>
+      </c>
+      <c r="B52">
         <f t="shared" si="11"/>
-        <v>2017-12-31</v>
+        <v>0</v>
       </c>
       <c r="C52" s="3" t="e">
         <f t="shared" si="12"/>
         <v>#DIV/0!</v>
       </c>
       <c r="F52" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="G52" s="5" t="e">
         <f>SLOPE(C50:C59,A50:A59)/C50/9</f>
@@ -5193,11 +5151,11 @@
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53">
         <f t="shared" si="13"/>
-        <v>2018</v>
-      </c>
-      <c r="B53" t="str">
+        <v>1900</v>
+      </c>
+      <c r="B53">
         <f t="shared" si="11"/>
-        <v>2018-12-31</v>
+        <v>0</v>
       </c>
       <c r="C53" s="3" t="e">
         <f t="shared" si="12"/>
@@ -5207,39 +5165,39 @@
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54">
         <f t="shared" si="13"/>
-        <v>2019</v>
-      </c>
-      <c r="B54" t="str">
+        <v>1900</v>
+      </c>
+      <c r="B54">
         <f t="shared" si="11"/>
-        <v>2019-12-31</v>
+        <v>0</v>
       </c>
       <c r="C54" s="3" t="e">
         <f t="shared" si="12"/>
         <v>#DIV/0!</v>
       </c>
       <c r="F54" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="G54" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55">
         <f t="shared" si="13"/>
-        <v>2020</v>
-      </c>
-      <c r="B55" t="str">
+        <v>1900</v>
+      </c>
+      <c r="B55">
         <f t="shared" si="11"/>
-        <v>2020-12-31</v>
+        <v>0</v>
       </c>
       <c r="C55" s="3" t="e">
         <f t="shared" si="12"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="F55" t="str">
+      <c r="F55">
         <f>B59</f>
-        <v>2024-09-30</v>
+        <v>0</v>
       </c>
       <c r="G55" s="3" t="e">
         <f>MIN(E12,G27,H44)*1.1</f>
@@ -5249,11 +5207,11 @@
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56">
         <f t="shared" si="13"/>
-        <v>2021</v>
-      </c>
-      <c r="B56" t="str">
+        <v>1900</v>
+      </c>
+      <c r="B56">
         <f t="shared" si="11"/>
-        <v>2021-12-31</v>
+        <v>0</v>
       </c>
       <c r="C56" s="3" t="e">
         <f t="shared" si="12"/>
@@ -5263,11 +5221,11 @@
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57">
         <f t="shared" si="13"/>
-        <v>2022</v>
-      </c>
-      <c r="B57" t="str">
+        <v>1900</v>
+      </c>
+      <c r="B57">
         <f t="shared" si="11"/>
-        <v>2022-12-31</v>
+        <v>0</v>
       </c>
       <c r="C57" s="3" t="e">
         <f t="shared" si="12"/>
@@ -5277,11 +5235,11 @@
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58">
         <f t="shared" si="13"/>
-        <v>2023</v>
-      </c>
-      <c r="B58" t="str">
+        <v>1900</v>
+      </c>
+      <c r="B58">
         <f t="shared" si="11"/>
-        <v>2023-12-31</v>
+        <v>0</v>
       </c>
       <c r="C58" s="3" t="e">
         <f t="shared" si="12"/>
@@ -5291,11 +5249,11 @@
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59">
         <f t="shared" si="13"/>
-        <v>2024</v>
-      </c>
-      <c r="B59" t="str">
+        <v>1900</v>
+      </c>
+      <c r="B59">
         <f t="shared" si="11"/>
-        <v>2024-09-30</v>
+        <v>0</v>
       </c>
       <c r="C59" s="3" t="e">
         <f t="shared" si="12"/>
@@ -5305,10 +5263,10 @@
     <row r="61" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B62" s="65" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="C62" s="118" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="D62" s="119"/>
       <c r="E62" s="119"/>
@@ -5334,9 +5292,9 @@
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B64" s="66" t="str">
+      <c r="B64" s="66">
         <f t="shared" ref="B64:B72" si="14">B3</f>
-        <v>2015-12-31</v>
+        <v>0</v>
       </c>
       <c r="C64" s="59" t="e">
         <f t="shared" ref="C64:C72" si="15">(E4-E3)/E3</f>
@@ -5356,9 +5314,9 @@
       </c>
     </row>
     <row r="65" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B65" s="66" t="str">
+      <c r="B65" s="66">
         <f t="shared" si="14"/>
-        <v>2016-12-31</v>
+        <v>0</v>
       </c>
       <c r="C65" s="54" t="e">
         <f t="shared" si="15"/>
@@ -5378,9 +5336,9 @@
       </c>
     </row>
     <row r="66" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B66" s="66" t="str">
+      <c r="B66" s="66">
         <f t="shared" si="14"/>
-        <v>2017-12-31</v>
+        <v>0</v>
       </c>
       <c r="C66" s="54" t="e">
         <f t="shared" si="15"/>
@@ -5400,9 +5358,9 @@
       </c>
     </row>
     <row r="67" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B67" s="66" t="str">
+      <c r="B67" s="66">
         <f t="shared" si="14"/>
-        <v>2018-12-31</v>
+        <v>0</v>
       </c>
       <c r="C67" s="54" t="e">
         <f t="shared" si="15"/>
@@ -5422,9 +5380,9 @@
       </c>
     </row>
     <row r="68" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B68" s="66" t="str">
+      <c r="B68" s="66">
         <f t="shared" si="14"/>
-        <v>2019-12-31</v>
+        <v>0</v>
       </c>
       <c r="C68" s="54" t="e">
         <f t="shared" si="15"/>
@@ -5444,9 +5402,9 @@
       </c>
     </row>
     <row r="69" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B69" s="66" t="str">
+      <c r="B69" s="66">
         <f t="shared" si="14"/>
-        <v>2020-12-31</v>
+        <v>0</v>
       </c>
       <c r="C69" s="54" t="e">
         <f t="shared" si="15"/>
@@ -5466,9 +5424,9 @@
       </c>
     </row>
     <row r="70" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B70" s="66" t="str">
+      <c r="B70" s="66">
         <f t="shared" si="14"/>
-        <v>2021-12-31</v>
+        <v>0</v>
       </c>
       <c r="C70" s="54" t="e">
         <f t="shared" si="15"/>
@@ -5488,9 +5446,9 @@
       </c>
     </row>
     <row r="71" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B71" s="66" t="str">
+      <c r="B71" s="66">
         <f t="shared" si="14"/>
-        <v>2022-12-31</v>
+        <v>0</v>
       </c>
       <c r="C71" s="54" t="e">
         <f t="shared" si="15"/>
@@ -5510,9 +5468,9 @@
       </c>
     </row>
     <row r="72" spans="2:6" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B72" s="67" t="str">
+      <c r="B72" s="67">
         <f t="shared" si="14"/>
-        <v>2023-12-31</v>
+        <v>0</v>
       </c>
       <c r="C72" s="56" t="e">
         <f t="shared" si="15"/>

</xml_diff>

<commit_message>
replace template. add abs() to denominator
</commit_message>
<xml_diff>
--- a/FCF_Analysis_Temp1.xlsx
+++ b/FCF_Analysis_Temp1.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AsusWebStorage\ran@benhur.co\MySyncFolder\python\investingAnalysis\financial_to_exel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AsusWebStorage\ran@benhur.co\MySyncFolder\RaniStuff\IBI\Stock Analysis\Financials\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50CF032B-85B3-44E4-ACAC-C39092318950}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22412FE6-D661-4C48-9528-179E7271A528}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1106,18 +1106,25 @@
     <xf numFmtId="166" fontId="0" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1125,13 +1132,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3493,14 +3493,14 @@
         <f>'FCF DATA'!G49</f>
         <v>Growth</v>
       </c>
-      <c r="F3" s="110" t="s">
+      <c r="F3" s="106" t="s">
         <v>22</v>
       </c>
-      <c r="G3" s="111"/>
-      <c r="I3" s="117" t="s">
+      <c r="G3" s="107"/>
+      <c r="I3" s="112" t="s">
         <v>23</v>
       </c>
-      <c r="J3" s="111"/>
+      <c r="J3" s="107"/>
     </row>
     <row r="4" spans="2:14" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C4" s="8" t="str">
@@ -3560,14 +3560,14 @@
         <f>'FCF DATA'!G54</f>
         <v>Min CF + 10%</v>
       </c>
-      <c r="F8" s="110" t="s">
+      <c r="F8" s="106" t="s">
         <v>26</v>
       </c>
-      <c r="G8" s="111"/>
-      <c r="I8" s="112" t="s">
+      <c r="G8" s="107"/>
+      <c r="I8" s="115" t="s">
         <v>27</v>
       </c>
-      <c r="J8" s="111"/>
+      <c r="J8" s="107"/>
     </row>
     <row r="9" spans="2:14" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C9" s="32">
@@ -3625,7 +3625,7 @@
       <c r="M11" s="14">
         <v>10</v>
       </c>
-      <c r="N11" s="113" t="s">
+      <c r="N11" s="116" t="s">
         <v>29</v>
       </c>
     </row>
@@ -3677,7 +3677,7 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="N12" s="114"/>
+      <c r="N12" s="117"/>
     </row>
     <row r="13" spans="2:14" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B13" s="13" t="s">
@@ -3733,10 +3733,10 @@
       </c>
     </row>
     <row r="14" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B14" s="108" t="s">
+      <c r="B14" s="110" t="s">
         <v>32</v>
       </c>
-      <c r="C14" s="109"/>
+      <c r="C14" s="111"/>
       <c r="D14" s="16">
         <f>$G$4</f>
         <v>0.12</v>
@@ -3780,10 +3780,10 @@
       <c r="N14" s="12"/>
     </row>
     <row r="15" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B15" s="108" t="s">
+      <c r="B15" s="110" t="s">
         <v>33</v>
       </c>
-      <c r="C15" s="109"/>
+      <c r="C15" s="111"/>
       <c r="D15" s="17">
         <f t="shared" ref="D15:M15" si="2">(1+$G$9)^D11</f>
         <v>1.1000000000000001</v>
@@ -3827,10 +3827,10 @@
       <c r="N15" s="12"/>
     </row>
     <row r="16" spans="2:14" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="115" t="s">
+      <c r="B16" s="108" t="s">
         <v>34</v>
       </c>
-      <c r="C16" s="116"/>
+      <c r="C16" s="109"/>
       <c r="D16" s="20" t="e">
         <f t="shared" ref="D16:M16" si="3">D13/D15</f>
         <v>#DIV/0!</v>
@@ -3896,11 +3896,11 @@
       <c r="D18" s="38"/>
     </row>
     <row r="19" spans="2:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C19" s="106" t="e" vm="4">
+      <c r="C19" s="113" t="e" vm="4">
         <f t="array" ref="C19">_FV('Data Entry'!C2,"Official name",TRUE)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="D19" s="107"/>
+      <c r="D19" s="114"/>
     </row>
     <row r="20" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C20" s="27" t="s">
@@ -3950,6 +3950,7 @@
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="N11:N12"/>
     <mergeCell ref="F3:G3"/>
     <mergeCell ref="B16:C16"/>
     <mergeCell ref="B15:C15"/>
@@ -3958,7 +3959,6 @@
     <mergeCell ref="B14:C14"/>
     <mergeCell ref="F8:G8"/>
     <mergeCell ref="I8:J8"/>
-    <mergeCell ref="N11:N12"/>
   </mergeCells>
   <conditionalFormatting sqref="D26">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="lessThan">
@@ -3977,7 +3977,7 @@
   <dimension ref="A1:O72"/>
   <sheetViews>
     <sheetView topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="G52" sqref="G52"/>
+      <selection activeCell="G53" sqref="G53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5102,7 +5102,7 @@
         <v>67</v>
       </c>
       <c r="G50" s="5" t="e">
-        <f>SLOPE(C56:C59,A56:A59)/C56/3</f>
+        <f>SLOPE(C56:C59,A56:A59)/ABS(C56)/3</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -5123,7 +5123,7 @@
         <v>68</v>
       </c>
       <c r="G51" s="5" t="e">
-        <f>SLOPE(C54:C59,A54:A59)/C54/5</f>
+        <f>SLOPE(C54:C59,A54:A59)/ABS(C54)/5</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -5144,7 +5144,7 @@
         <v>69</v>
       </c>
       <c r="G52" s="5" t="e">
-        <f>SLOPE(C50:C59,A50:A59)/C50/9</f>
+        <f>SLOPE(C50:C59,A50:A59)/ABS(C50)/9</f>
         <v>#DIV/0!</v>
       </c>
     </row>

</xml_diff>